<commit_message>
New Code with API
</commit_message>
<xml_diff>
--- a/Selenium-Scripts/src/Testdata.xlsx
+++ b/Selenium-Scripts/src/Testdata.xlsx
@@ -5,19 +5,19 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\ECom\EcomFramework\Framework\Selenium-Scripts\src\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation Projects\Automation Framework\Automation_Framework\Selenium-Scripts\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15945" windowHeight="2670" tabRatio="701" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15945" windowHeight="2670" tabRatio="701" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="SetUp" sheetId="34" r:id="rId1"/>
     <sheet name="HomePage" sheetId="37" r:id="rId2"/>
     <sheet name="SearchPage" sheetId="38" r:id="rId3"/>
     <sheet name="Sheet1" sheetId="41" r:id="rId4"/>
-    <sheet name="Products" sheetId="35" r:id="rId5"/>
-    <sheet name="checkOut" sheetId="39" r:id="rId6"/>
+    <sheet name="PDP" sheetId="35" r:id="rId5"/>
+    <sheet name="Checkout" sheetId="39" r:id="rId6"/>
     <sheet name="ShipperForm" sheetId="40" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="48">
   <si>
     <t>Key</t>
   </si>
@@ -57,27 +57,18 @@
     <t>Searchproduct</t>
   </si>
   <si>
-    <t>selectProduct</t>
-  </si>
-  <si>
     <t>productPrice</t>
   </si>
   <si>
     <t>styleNo</t>
   </si>
   <si>
-    <t>oneProduct</t>
-  </si>
-  <si>
     <t>Mary Kay | Official Site</t>
   </si>
   <si>
     <t>appConfigFileMaryKay</t>
   </si>
   <si>
-    <t>zipCode</t>
-  </si>
-  <si>
     <t>99501</t>
   </si>
   <si>
@@ -91,9 +82,6 @@
   </si>
   <si>
     <t>Guest Checkout</t>
-  </si>
-  <si>
-    <t>GuestCheckOutPage</t>
   </si>
   <si>
     <t>searchResult</t>
@@ -161,6 +149,27 @@
   </si>
   <si>
     <t>abc@1234</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>productCount</t>
+  </si>
+  <si>
+    <t>guestChek-Out</t>
+  </si>
+  <si>
+    <t>ZipCode</t>
+  </si>
+  <si>
+    <t>guestCheckOutHeading</t>
+  </si>
+  <si>
+    <t>checkOutbtn</t>
+  </si>
+  <si>
+    <t>Checkout</t>
   </si>
 </sst>
 </file>
@@ -594,7 +603,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +634,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
@@ -663,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -675,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,15 +707,15 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -738,18 +747,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -766,7 +775,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,36 +806,36 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -839,10 +848,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,18 +870,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -882,10 +907,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -904,66 +929,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B9" s="12" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>